<commit_message>
MàJ des fichiers ProgressiveCurve (ajout temps de mesure et substrat utilisé) et Endpoint assay (ajout enzyme utilisée).
</commit_message>
<xml_diff>
--- a/script/template_gen/endpointassay.xlsx
+++ b/script/template_gen/endpointassay.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="95">
   <si>
     <t>AnalysisDate</t>
   </si>
@@ -83,6 +83,9 @@
     <t>MeasuredMetabolite</t>
   </si>
   <si>
+    <t>UsedEnzyme</t>
+  </si>
+  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -150,6 +153,9 @@
   </si>
   <si>
     <t># Métabolite dosé</t>
+  </si>
+  <si>
+    <t># Enzyme utilisée</t>
   </si>
   <si>
     <t># Commentaire</t>
@@ -198,7 +204,7 @@
     <t># format: texte, à définir....</t>
   </si>
   <si>
-    <t># format: nombre entier, ne pas spécifier d'unité</t>
+    <t># format: nombre entier, ne pas spécifier d'unité (nm)</t>
   </si>
   <si>
     <t># format: alphanumérique XXXX-XXXX,  ne pas spécifier d'unité</t>
@@ -286,6 +292,9 @@
   </si>
   <si>
     <t># ex: glucose</t>
+  </si>
+  <si>
+    <t># ex:</t>
   </si>
   <si>
     <t/>
@@ -333,7 +342,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -412,301 +421,316 @@
       <c r="X1" t="s">
         <v>23</v>
       </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="R2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="S2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="V2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="W2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="X2" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="M3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="N3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="P3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="Q3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="R3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="S3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="T3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="U3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="V3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="W3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="X3" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" t="s">
+        <v>64</v>
+      </c>
+      <c r="L4" t="s">
         <v>61</v>
       </c>
-      <c r="K4" t="s">
-        <v>62</v>
-      </c>
-      <c r="L4" t="s">
-        <v>59</v>
-      </c>
       <c r="M4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="P4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Q4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="R4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="S4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="U4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="V4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="W4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="X4" t="s">
-        <v>68</v>
+        <v>61</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="J5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="M5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="N5" t="s">
+        <v>84</v>
+      </c>
+      <c r="O5" t="s">
+        <v>85</v>
+      </c>
+      <c r="P5" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>87</v>
+      </c>
+      <c r="R5" t="s">
+        <v>88</v>
+      </c>
+      <c r="S5" t="s">
+        <v>89</v>
+      </c>
+      <c r="T5" t="s">
+        <v>90</v>
+      </c>
+      <c r="U5" t="s">
+        <v>91</v>
+      </c>
+      <c r="V5" t="s">
         <v>82</v>
       </c>
-      <c r="O5" t="s">
-        <v>83</v>
-      </c>
-      <c r="P5" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>85</v>
-      </c>
-      <c r="R5" t="s">
-        <v>86</v>
-      </c>
-      <c r="S5" t="s">
-        <v>87</v>
-      </c>
-      <c r="T5" t="s">
-        <v>88</v>
-      </c>
-      <c r="U5" t="s">
-        <v>89</v>
-      </c>
-      <c r="V5" t="s">
-        <v>80</v>
-      </c>
       <c r="W5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="X5" t="s">
-        <v>91</v>
+        <v>93</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>